<commit_message>
feat: Update Issue 1 (Deposit an Product)
</commit_message>
<xml_diff>
--- a/public/template/report/Template_Report_Deposit_Summary.xlsx
+++ b/public/template/report/Template_Report_Deposit_Summary.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E43112-AE8D-4CD4-A311-4E1E736C288D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5046A-5633-40C7-9CA7-F697BAA9B629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report Growth" sheetId="1" r:id="rId1"/>
+    <sheet name="Report Summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,13 +30,13 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Remaining</t>
+    <t>Return (Rp)</t>
   </si>
   <si>
-    <t>Return</t>
+    <t>Used (Rp)</t>
   </si>
   <si>
-    <t>Used</t>
+    <t>Remaining (Rp)</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -459,13 +459,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="1"/>

</xml_diff>